<commit_message>
UM-1/4 TC's updated with the below fixes UM1-ADMN045 & ADMN128, UM4-ADMN065B, ADMN081b & ADMN103B
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/AssetNameTestData.xlsx
+++ b/src/test/resources/TestData/AssetNameTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj.ghadei\git\VRT\VRT\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruchika.Behura\git\VRT\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F9E082-73B0-4759-B6D6-B50078A21817}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2155C27E-AE7D-4236-BED3-303D3B797698}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="270" windowWidth="20460" windowHeight="10800" tabRatio="847" firstSheet="23" activeTab="32" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="847" firstSheet="32" activeTab="40" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
   </bookViews>
   <sheets>
     <sheet name="ASST02" sheetId="2" r:id="rId1"/>
@@ -48,6 +48,12 @@
     <sheet name="ASSTHB012a" sheetId="41" r:id="rId33"/>
     <sheet name="ASSTHB012b" sheetId="44" r:id="rId34"/>
     <sheet name="testAsset" sheetId="43" r:id="rId35"/>
+    <sheet name="ASST024_1STP" sheetId="45" r:id="rId36"/>
+    <sheet name="ASST024_1A" sheetId="46" r:id="rId37"/>
+    <sheet name="ASST024_2STP" sheetId="47" r:id="rId38"/>
+    <sheet name="ASST024_2ASTP" sheetId="48" r:id="rId39"/>
+    <sheet name="ASST019STP" sheetId="49" r:id="rId40"/>
+    <sheet name="ASST027STP" sheetId="50" r:id="rId41"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1948,7 +1954,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4681" uniqueCount="1220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4752" uniqueCount="1271">
   <si>
     <t>Name</t>
   </si>
@@ -5608,13 +5614,166 @@
   </si>
   <si>
     <t>10/26/2017</t>
+  </si>
+  <si>
+    <t>Snum</t>
+  </si>
+  <si>
+    <t>Rnum</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>AB12</t>
+  </si>
+  <si>
+    <t>12_A</t>
+  </si>
+  <si>
+    <t>AB?</t>
+  </si>
+  <si>
+    <t>1A/</t>
+  </si>
+  <si>
+    <t>2B\</t>
+  </si>
+  <si>
+    <t>12.AB</t>
+  </si>
+  <si>
+    <t>a  b  c1</t>
+  </si>
+  <si>
+    <t>2~</t>
+  </si>
+  <si>
+    <t>AB`</t>
+  </si>
+  <si>
+    <t>12!</t>
+  </si>
+  <si>
+    <t>AB@</t>
+  </si>
+  <si>
+    <t>1A#</t>
+  </si>
+  <si>
+    <t>2B$%</t>
+  </si>
+  <si>
+    <t>vb^</t>
+  </si>
+  <si>
+    <t>fg&amp;1</t>
+  </si>
+  <si>
+    <t>qw*</t>
+  </si>
+  <si>
+    <t>2w+</t>
+  </si>
+  <si>
+    <t>r5=</t>
+  </si>
+  <si>
+    <t>t6{[}]</t>
+  </si>
+  <si>
+    <t>7qw|</t>
+  </si>
+  <si>
+    <t>5r:;</t>
+  </si>
+  <si>
+    <t>aw"'&lt;,&gt;</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>12-A</t>
+  </si>
+  <si>
+    <t>AB1</t>
+  </si>
+  <si>
+    <t>AC2</t>
+  </si>
+  <si>
+    <t>BA3</t>
+  </si>
+  <si>
+    <t>BB4</t>
+  </si>
+  <si>
+    <t>CC5</t>
+  </si>
+  <si>
+    <t>45A</t>
+  </si>
+  <si>
+    <t>A-1</t>
+  </si>
+  <si>
+    <t>a  b  c</t>
+  </si>
+  <si>
+    <t>q&amp;*</t>
+  </si>
+  <si>
+    <t>$#%%</t>
+  </si>
+  <si>
+    <t>1  A#</t>
+  </si>
+  <si>
+    <t>fg  1</t>
+  </si>
+  <si>
+    <t>1q</t>
+  </si>
+  <si>
+    <t>qw*()</t>
+  </si>
+  <si>
+    <t>SetupName</t>
+  </si>
+  <si>
+    <t>SensorCount</t>
+  </si>
+  <si>
+    <t>TempCount</t>
+  </si>
+  <si>
+    <t>TCSensorLabel</t>
+  </si>
+  <si>
+    <t>Qstart</t>
+  </si>
+  <si>
+    <t>ASST019STP</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>abc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5649,8 +5808,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5672,6 +5839,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5711,10 +5890,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -5732,8 +5912,29 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -12138,7 +12339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F849282-884D-43B5-AC4C-35EA751A7EE8}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -19621,6 +19822,449 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EF90128-5E85-4A3C-9BEB-DE447876A8FF}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B2" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
+        <v>123</v>
+      </c>
+      <c r="B3" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>1223</v>
+      </c>
+      <c r="B4" s="18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B5" s="18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B6" s="18">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B7" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B8" s="18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B9" s="18">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D06728-46DC-451D-97DC-0DCBF8C96104}">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B2" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B3" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B4" s="18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B5" s="18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B6" s="18">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B7" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B8" s="18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B9" s="18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B10" s="18">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B11" s="18">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B13" s="18">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B14" s="18">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B15" s="18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B16" s="18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B17" s="18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B18" s="18">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{E6C3D314-ADCD-4025-B48D-1F78CD5B3223}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F885FD-1FF7-4875-B905-EA1FDA89DE03}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B2" s="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B3" s="18">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B4" s="18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B5" s="18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B6" s="18">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B7" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B8" s="18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B9" s="18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B10" s="13">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31752241-E35E-41F6-9BD0-F587CF664CC7}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{66C29E9B-2533-49F9-B52C-ADB68C2887B3}"/>
+    <hyperlink ref="B5" r:id="rId2" display="12!!!@" xr:uid="{4F9A5AA8-293D-4E0F-B8A8-E874EE6EA9A9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0CA098D-760A-4887-9AC3-050D72D6661B}">
   <dimension ref="A1:H27"/>
@@ -20346,6 +20990,86 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B4D6E5-D0B5-4085-AA8C-2F4DB91423EA}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1263</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1264</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1266</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1267</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDEEAC7D-06A4-4075-B7D2-CBB6553C7070}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
VRT Project updated , with Asset Details & Multiple User creation script changes.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/AssetNameTestData.xlsx
+++ b/src/test/resources/TestData/AssetNameTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruchika.Behura\git\VRT\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2155C27E-AE7D-4236-BED3-303D3B797698}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD225B11-574C-4601-A57B-9B5C64A458D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="847" firstSheet="32" activeTab="40" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="847" firstSheet="32" activeTab="39" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
   </bookViews>
   <sheets>
     <sheet name="ASST02" sheetId="2" r:id="rId1"/>
@@ -1954,7 +1954,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4752" uniqueCount="1271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4746" uniqueCount="1270">
   <si>
     <t>Name</t>
   </si>
@@ -5707,9 +5707,6 @@
   </si>
   <si>
     <t>BB4</t>
-  </si>
-  <si>
-    <t>CC5</t>
   </si>
   <si>
     <t>45A</t>
@@ -20073,10 +20070,10 @@
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F885FD-1FF7-4875-B905-EA1FDA89DE03}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20111,54 +20108,6 @@
       </c>
       <c r="B4" s="18">
         <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>1248</v>
-      </c>
-      <c r="B5" s="18">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>1249</v>
-      </c>
-      <c r="B6" s="18">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>1250</v>
-      </c>
-      <c r="B7" s="18">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>1251</v>
-      </c>
-      <c r="B8" s="18">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>1252</v>
-      </c>
-      <c r="B9" s="18">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>1253</v>
-      </c>
-      <c r="B10" s="13">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -20189,7 +20138,7 @@
         <v>1245</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -20197,7 +20146,7 @@
         <v>1246</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -20213,7 +20162,7 @@
         <v>1248</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -20229,12 +20178,12 @@
         <v>1250</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>1236</v>
@@ -20242,18 +20191,18 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>1259</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>1260</v>
       </c>
     </row>
   </sheetData>
@@ -20997,8 +20946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B4D6E5-D0B5-4085-AA8C-2F4DB91423EA}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21008,36 +20957,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>1261</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="5" t="s">
         <v>1262</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>1263</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="25" t="s">
         <v>1264</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>1265</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>1266</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" t="s">
         <v>1267</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1268</v>
       </c>
     </row>
   </sheetData>
@@ -21049,7 +20998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDEEAC7D-06A4-4075-B7D2-CBB6553C7070}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -21060,12 +21009,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Asset Details 1&2 scripts with all bugs Fixed except AD2 with ASST010,ASST011 pending
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/AssetNameTestData.xlsx
+++ b/src/test/resources/TestData/AssetNameTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SSC\git\VRT\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78561573-64E8-49B0-B10D-A67D509F5420}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694F95A2-E4B8-4C34-A6FE-85E503747E42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="847" firstSheet="30" activeTab="33" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="847" activeTab="5" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
   </bookViews>
   <sheets>
     <sheet name="ASST02" sheetId="2" r:id="rId1"/>
@@ -1247,7 +1247,7 @@
     <author>Ghadei, Manoj (Amphenol-AS)</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{8F94AA8B-8249-4FB6-9235-5F572816D7E6}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{8F94AA8B-8249-4FB6-9235-5F572816D7E6}">
       <text>
         <r>
           <rPr>
@@ -1993,7 +1993,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5407" uniqueCount="1572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5389" uniqueCount="1579">
   <si>
     <t>Name</t>
   </si>
@@ -6709,6 +6709,27 @@
   </si>
   <si>
     <t>ASSTHB0200</t>
+  </si>
+  <si>
+    <t>Aname</t>
+  </si>
+  <si>
+    <t>AID</t>
+  </si>
+  <si>
+    <t>AType</t>
+  </si>
+  <si>
+    <t>AManufaturer</t>
+  </si>
+  <si>
+    <t>ALocation</t>
+  </si>
+  <si>
+    <t>ASST025STP</t>
+  </si>
+  <si>
+    <t>Aas</t>
   </si>
 </sst>
 </file>
@@ -12783,7 +12804,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D3" sqref="D3:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12822,7 +12843,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -12845,7 +12866,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -12868,7 +12889,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -12891,7 +12912,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -12914,7 +12935,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
@@ -12937,7 +12958,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
@@ -12960,7 +12981,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -12983,7 +13004,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -14387,7 +14408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B08DF299-26FC-4816-95E4-0F0D7AAB6D5B}">
   <dimension ref="A1:M201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+    <sheetView topLeftCell="A145" workbookViewId="0">
       <selection activeCell="L159" sqref="L159"/>
     </sheetView>
   </sheetViews>
@@ -23826,59 +23847,91 @@
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184DA8F5-6C11-4DB9-BB7A-EC50ADFF9EE3}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>1573</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>1574</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>1575</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>1576</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>1242</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>1243</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>1244</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>1245</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="J1" s="24" t="s">
         <v>1246</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="K1" s="24" t="s">
         <v>1251</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>1577</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1578</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>1254</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="G2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>1247</v>
       </c>
-      <c r="E2" t="s">
+      <c r="J2" t="s">
         <v>1252</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>1253</v>
       </c>
     </row>
@@ -24024,7 +24077,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="D3" sqref="D3:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24063,7 +24116,7 @@
         <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -24086,7 +24139,7 @@
         <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -24109,7 +24162,7 @@
         <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -24132,7 +24185,7 @@
         <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -24155,7 +24208,7 @@
         <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
@@ -24178,7 +24231,7 @@
         <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
@@ -24201,7 +24254,7 @@
         <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -24224,7 +24277,7 @@
         <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -24243,11 +24296,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C599F558-8C31-43A4-A408-30DBEA8C34EE}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24258,10 +24311,9 @@
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="81.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -24280,25 +24332,19 @@
       <c r="F1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>48</v>
+        <v>153</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>48</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
         <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -24306,25 +24352,19 @@
       <c r="F2" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="3">
-        <v>5</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>48</v>
+        <v>153</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>48</v>
+        <v>152</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -24332,25 +24372,19 @@
       <c r="F3" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="3">
-        <v>5</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>48</v>
+        <v>153</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>48</v>
+        <v>152</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -24358,25 +24392,19 @@
       <c r="F4" t="s">
         <v>147</v>
       </c>
-      <c r="G4" s="3">
-        <v>5</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>48</v>
+        <v>153</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>48</v>
+        <v>152</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -24384,25 +24412,19 @@
       <c r="F5" t="s">
         <v>147</v>
       </c>
-      <c r="G5" s="3">
-        <v>5</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>48</v>
+        <v>153</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>48</v>
+        <v>152</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
@@ -24410,25 +24432,19 @@
       <c r="F6" t="s">
         <v>147</v>
       </c>
-      <c r="G6" s="3">
-        <v>5</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>48</v>
+        <v>153</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>48</v>
+        <v>152</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
@@ -24436,14 +24452,8 @@
       <c r="F7" t="s">
         <v>147</v>
       </c>
-      <c r="G7" s="3">
-        <v>5</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>153</v>
       </c>
@@ -24454,7 +24464,7 @@
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -24462,14 +24472,8 @@
       <c r="F8" t="s">
         <v>147</v>
       </c>
-      <c r="G8" s="3">
-        <v>5</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>153</v>
       </c>
@@ -24480,7 +24484,7 @@
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -24488,14 +24492,8 @@
       <c r="F9" t="s">
         <v>147</v>
       </c>
-      <c r="G9" s="3">
-        <v>5</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>153</v>
       </c>
@@ -24506,7 +24504,7 @@
         <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -24514,14 +24512,8 @@
       <c r="F10" t="s">
         <v>147</v>
       </c>
-      <c r="G10" s="3">
-        <v>5</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>153</v>
       </c>
@@ -24532,7 +24524,7 @@
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
@@ -24540,14 +24532,8 @@
       <c r="F11" t="s">
         <v>147</v>
       </c>
-      <c r="G11" s="3">
-        <v>5</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>153</v>
       </c>
@@ -24558,7 +24544,7 @@
         <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
@@ -24566,14 +24552,8 @@
       <c r="F12" t="s">
         <v>147</v>
       </c>
-      <c r="G12" s="3">
-        <v>5</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>153</v>
       </c>
@@ -24584,7 +24564,7 @@
         <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
@@ -24592,14 +24572,8 @@
       <c r="F13" t="s">
         <v>147</v>
       </c>
-      <c r="G13" s="3">
-        <v>5</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>153</v>
       </c>
@@ -24610,7 +24584,7 @@
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
@@ -24618,14 +24592,8 @@
       <c r="F14" t="s">
         <v>147</v>
       </c>
-      <c r="G14" s="3">
-        <v>5</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>153</v>
       </c>
@@ -24636,7 +24604,7 @@
         <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
@@ -24644,14 +24612,8 @@
       <c r="F15" t="s">
         <v>147</v>
       </c>
-      <c r="G15" s="3">
-        <v>5</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>153</v>
       </c>
@@ -24662,7 +24624,7 @@
         <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E16" t="s">
         <v>7</v>
@@ -24670,14 +24632,8 @@
       <c r="F16" t="s">
         <v>147</v>
       </c>
-      <c r="G16" s="3">
-        <v>5</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>153</v>
       </c>
@@ -24688,7 +24644,7 @@
         <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
@@ -24696,14 +24652,8 @@
       <c r="F17" t="s">
         <v>147</v>
       </c>
-      <c r="G17" s="3">
-        <v>5</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>153</v>
       </c>
@@ -24714,7 +24664,7 @@
         <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E18" t="s">
         <v>7</v>
@@ -24722,14 +24672,8 @@
       <c r="F18" t="s">
         <v>147</v>
       </c>
-      <c r="G18" s="3">
-        <v>5</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>153</v>
       </c>
@@ -24740,7 +24684,7 @@
         <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E19" t="s">
         <v>7</v>
@@ -24748,14 +24692,8 @@
       <c r="F19" t="s">
         <v>147</v>
       </c>
-      <c r="G19" s="3">
-        <v>5</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>153</v>
       </c>
@@ -24766,7 +24704,7 @@
         <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E20" t="s">
         <v>7</v>
@@ -24774,14 +24712,8 @@
       <c r="F20" t="s">
         <v>147</v>
       </c>
-      <c r="G20" s="3">
-        <v>5</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>153</v>
       </c>
@@ -24792,7 +24724,7 @@
         <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E21" t="s">
         <v>7</v>
@@ -24800,14 +24732,8 @@
       <c r="F21" t="s">
         <v>147</v>
       </c>
-      <c r="G21" s="3">
-        <v>5</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>153</v>
       </c>
@@ -24818,7 +24744,7 @@
         <v>31</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E22" t="s">
         <v>7</v>
@@ -24826,14 +24752,8 @@
       <c r="F22" t="s">
         <v>147</v>
       </c>
-      <c r="G22" s="3">
-        <v>5</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>153</v>
       </c>
@@ -24844,7 +24764,7 @@
         <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E23" t="s">
         <v>7</v>
@@ -24852,14 +24772,8 @@
       <c r="F23" t="s">
         <v>147</v>
       </c>
-      <c r="G23" s="3">
-        <v>5</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>153</v>
       </c>
@@ -24870,7 +24784,7 @@
         <v>34</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E24" t="s">
         <v>7</v>
@@ -24878,14 +24792,8 @@
       <c r="F24" t="s">
         <v>147</v>
       </c>
-      <c r="G24" s="3">
-        <v>5</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>153</v>
       </c>
@@ -24896,7 +24804,7 @@
         <v>37</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E25" t="s">
         <v>7</v>
@@ -24904,14 +24812,8 @@
       <c r="F25" t="s">
         <v>147</v>
       </c>
-      <c r="G25" s="3">
-        <v>5</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>153</v>
       </c>
@@ -24922,7 +24824,7 @@
         <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E26" t="s">
         <v>7</v>
@@ -24930,14 +24832,8 @@
       <c r="F26" t="s">
         <v>147</v>
       </c>
-      <c r="G26" s="3">
-        <v>5</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>153</v>
       </c>
@@ -24948,27 +24844,18 @@
         <v>35</v>
       </c>
       <c r="D27" t="s">
-        <v>6</v>
+        <v>1578</v>
       </c>
       <c r="E27" t="s">
         <v>7</v>
       </c>
       <c r="F27" t="s">
         <v>147</v>
-      </c>
-      <c r="G27" s="3">
-        <v>5</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="A2" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>